<commit_message>
Final version, average accuracy 98%!
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -53,6 +53,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -105,14 +108,51 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -120,14 +160,331 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="35">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Normal Find</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$B$12:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.9046</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.965</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9574</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9605</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9642</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Normal Repair</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$C$12:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.8607</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9326</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9564</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9601</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9531</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9954</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9957</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Hard Find</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$D$12:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.6163</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6954</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8466</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8254</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.695</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8928</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9671</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Hard Repair</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$E$12:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.5608</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6587</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6922</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.889</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9647</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2137517976"/>
+        <c:axId val="2088911992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2137517976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2088911992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2088911992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.45"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2137517976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.05"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1231900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -470,27 +827,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="3"/>
+      <c r="A2" s="6"/>
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -614,6 +971,278 @@
       <c r="J5">
         <v>870</v>
       </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>41602</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1390</v>
+      </c>
+      <c r="E6">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="F6">
+        <v>0.96020000000000005</v>
+      </c>
+      <c r="G6">
+        <v>739</v>
+      </c>
+      <c r="H6">
+        <v>0.82540000000000002</v>
+      </c>
+      <c r="I6">
+        <v>0.50470000000000004</v>
+      </c>
+      <c r="J6">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2">
+        <v>41611</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2034</v>
+      </c>
+      <c r="E7">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="F7">
+        <v>0.96009999999999995</v>
+      </c>
+      <c r="G7">
+        <v>747</v>
+      </c>
+      <c r="H7">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="I7">
+        <v>0.69220000000000004</v>
+      </c>
+      <c r="J7">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0.96419999999999995</v>
+      </c>
+      <c r="F8">
+        <v>0.95309999999999995</v>
+      </c>
+      <c r="H8">
+        <v>0.72</v>
+      </c>
+      <c r="I8">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="F9">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="H9">
+        <v>0.89280000000000004</v>
+      </c>
+      <c r="I9">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>41630</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.997</v>
+      </c>
+      <c r="F10">
+        <v>0.99570000000000003</v>
+      </c>
+      <c r="H10">
+        <v>0.96709999999999996</v>
+      </c>
+      <c r="I10">
+        <v>0.9647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0.90459999999999996</v>
+      </c>
+      <c r="C12">
+        <v>0.86070000000000002</v>
+      </c>
+      <c r="D12">
+        <v>0.61629999999999996</v>
+      </c>
+      <c r="E12">
+        <v>0.56079999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="C13">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="D13">
+        <v>0.69540000000000002</v>
+      </c>
+      <c r="E13">
+        <v>0.65869999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0.95740000000000003</v>
+      </c>
+      <c r="C14">
+        <v>0.95640000000000003</v>
+      </c>
+      <c r="D14">
+        <v>0.84660000000000002</v>
+      </c>
+      <c r="E14">
+        <v>0.59279999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.96020000000000005</v>
+      </c>
+      <c r="D15">
+        <v>0.82540000000000002</v>
+      </c>
+      <c r="E15">
+        <v>0.50470000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="C16">
+        <v>0.96009999999999995</v>
+      </c>
+      <c r="D16">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="E16">
+        <v>0.69220000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>0.96419999999999995</v>
+      </c>
+      <c r="C17">
+        <v>0.95309999999999995</v>
+      </c>
+      <c r="D17">
+        <v>0.72</v>
+      </c>
+      <c r="E17">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="C18">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="D18">
+        <v>0.89280000000000004</v>
+      </c>
+      <c r="E18">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>0.997</v>
+      </c>
+      <c r="C19">
+        <v>0.99570000000000003</v>
+      </c>
+      <c r="D19">
+        <v>0.96709999999999996</v>
+      </c>
+      <c r="E19">
+        <v>0.9647</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -625,6 +1254,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>